<commit_message>
(DWG 1100, DWG 1110, Sam's BOM)
1100 changed back orientation of cable to the right facing.
capatilized BOM of (Sam's BOM) & 1110
Fixed color for connectors of DWG 1100 & 1110
</commit_message>
<xml_diff>
--- a/docs/BOM(from sam).xlsx
+++ b/docs/BOM(from sam).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Samuel Mattingly\Documents\GitHub\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacko\OneDrive\Documents\Gallagher-Station-Duke-Energy-Museum-Exhibit\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEAE10A-EF71-4AC3-8D45-F830A1B6B85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB52251-8C82-4834-8A52-C33987B8AE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22776" yWindow="204" windowWidth="21576" windowHeight="11280" xr2:uid="{01FCA31E-F3D9-4F4A-B142-3532DA3C93F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01FCA31E-F3D9-4F4A-B142-3532DA3C93F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,9 +61,6 @@
     <t>J5</t>
   </si>
   <si>
-    <t>3-Pin  Male Molex Connector</t>
-  </si>
-  <si>
     <t>3-M-MOLEX</t>
   </si>
   <si>
@@ -94,12 +91,6 @@
     <t>288T232R161A1</t>
   </si>
   <si>
-    <t>Rotary Encoder</t>
-  </si>
-  <si>
-    <t>Servo Motor</t>
-  </si>
-  <si>
     <t>CABLE_001</t>
   </si>
   <si>
@@ -127,18 +118,6 @@
     <t>S4</t>
   </si>
   <si>
-    <t>NO-Push Button (Confirm Button)</t>
-  </si>
-  <si>
-    <t>NO-Push Button (Reset Button)</t>
-  </si>
-  <si>
-    <t>NO-Push Button (Send Power Button)</t>
-  </si>
-  <si>
-    <t>NO-Push Button (Phone Switch)</t>
-  </si>
-  <si>
     <t>PB-001</t>
   </si>
   <si>
@@ -187,24 +166,15 @@
     <t>2-M-MOLEX</t>
   </si>
   <si>
-    <t>2-Pin  Male Molex Connector</t>
-  </si>
-  <si>
     <t>DWG 1610 BILL OF MATERIALS (BOM)</t>
   </si>
   <si>
     <t>J37</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2-Pin Male Molex Connector</t>
-  </si>
-  <si>
     <t>DS1</t>
   </si>
   <si>
-    <t>60W LED Light-Bulb</t>
-  </si>
-  <si>
     <t>LED-60</t>
   </si>
   <si>
@@ -212,6 +182,36 @@
   </si>
   <si>
     <t>REFFERENCE DRAWING 1620</t>
+  </si>
+  <si>
+    <t>SERVO MOTOR</t>
+  </si>
+  <si>
+    <t>ROTARY ENCODER</t>
+  </si>
+  <si>
+    <t>3-PIN MALE MOLEX CONNECTOR</t>
+  </si>
+  <si>
+    <t>2-PIN MALE MOLEX CONNECTOR</t>
+  </si>
+  <si>
+    <t>NO-PUSH BUTTON (CONFIRM BUTTON)</t>
+  </si>
+  <si>
+    <t>NO-PUSH BUTTON (RESET BUTTON)</t>
+  </si>
+  <si>
+    <t>NO-PUSH BUTTON (SEND POWER BUTTON)</t>
+  </si>
+  <si>
+    <t>NO-PUSH BUTTON (PHONE SWITCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2-PIN MALE MOLEX CONNECTOR</t>
+  </si>
+  <si>
+    <t>60W LED LIGHT-BULB</t>
   </si>
 </sst>
 </file>
@@ -247,7 +247,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -343,44 +343,18 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -390,12 +364,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -423,17 +391,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -751,14 +714,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3266BBDC-8BF9-4EB0-AF9C-F59BD7AD69F0}">
   <dimension ref="B1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -781,167 +744,167 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
-        <v>15</v>
-      </c>
       <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>18</v>
+        <v>50</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="15"/>
+      <c r="B15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="10"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="13"/>
+      <c r="B16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="11"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -949,141 +912,141 @@
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>49</v>
+      <c r="B20" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>49</v>
+      <c r="B21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>49</v>
+      <c r="B22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>49</v>
+      <c r="B23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="12" t="s">
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="10"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="10"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="13" t="s">
+      <c r="C31" s="12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="12"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="12"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="12"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="13"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1091,44 +1054,44 @@
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>49</v>
+      <c r="B35" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>56</v>
+      <c r="B36" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="D37" s="20"/>
+      <c r="B37" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="11"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="22"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="22"/>
+      <c r="C39" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>